<commit_message>
Add bank failure classification by using MCES
</commit_message>
<xml_diff>
--- a/Experiment_Resulsts/Bank_Classification_Results_using_10_Features_5_fold.xlsx
+++ b/Experiment_Resulsts/Bank_Classification_Results_using_10_Features_5_fold.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DRTNTUN\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\htet_mces_bank_data\Experiment_Resulsts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA06BA25-0F89-454A-8CD2-E893157790BA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD142DB9-D12B-45B8-9BE7-71D880C1FB4D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{98666712-FD92-4C48-8ABF-24F5869146C3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="15">
   <si>
     <t>Last Record</t>
   </si>
@@ -105,18 +105,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -127,6 +121,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -143,17 +149,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -470,8 +478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3DCF0E0-FAAB-441A-A370-B138D481EADA}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -480,28 +488,28 @@
     <col min="7" max="7" width="11.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -620,51 +628,51 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>0.39567858735974698</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>8.8867149758454094</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>0.29504791131798702</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="5">
         <v>83.856682769726206</v>
       </c>
-      <c r="F9" s="3">
-        <v>0</v>
-      </c>
-      <c r="G9" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -783,57 +791,51 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="2">
         <v>0.39423882159092699</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="2">
         <v>9.2988515176374094</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="2">
         <v>0.20727884512710201</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="5">
         <v>84.104330708661394</v>
       </c>
-      <c r="F19" s="3">
-        <v>0</v>
-      </c>
-      <c r="G19" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="5" t="s">
+      <c r="F19" s="2">
+        <v>0</v>
+      </c>
+      <c r="G19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E22" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F22" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="G22" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -953,25 +955,25 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="2">
         <v>0.36149413571508499</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C29" s="2">
         <v>8.4134125636672294</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D29" s="2">
         <v>0.14006322537694299</v>
       </c>
-      <c r="E29" s="7">
+      <c r="E29" s="5">
         <v>86.638370118845501</v>
       </c>
-      <c r="F29" s="3">
-        <v>0</v>
-      </c>
-      <c r="G29" s="3">
+      <c r="F29" s="2">
+        <v>0</v>
+      </c>
+      <c r="G29" s="2">
         <v>0</v>
       </c>
     </row>

</xml_diff>